<commit_message>
Cleaned up FontTextureManager logic.
</commit_message>
<xml_diff>
--- a/TestCaseStatus.xlsx
+++ b/TestCaseStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{442FFDF3-8CEA-BB4E-9990-62D00A4689AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8608C38F-31AC-4A47-AE04-85490E8A5B24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="7840" windowWidth="28040" windowHeight="17440" xr2:uid="{835AE8E8-6B96-A741-AB6E-79E0122A2F31}"/>
+    <workbookView xWindow="8880" yWindow="2500" windowWidth="28040" windowHeight="17440" xr2:uid="{835AE8E8-6B96-A741-AB6E-79E0122A2F31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Test</t>
   </si>
@@ -177,16 +177,29 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Locations seem off sometimes</t>
+  </si>
+  <si>
+    <t>Labels not working</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,8 +233,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -540,7 +554,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,11 +607,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -617,8 +631,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -626,93 +640,129 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Geometry Manager working again. OBJ Model reader working again. Default labels working.
</commit_message>
<xml_diff>
--- a/TestCaseStatus.xlsx
+++ b/TestCaseStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8608C38F-31AC-4A47-AE04-85490E8A5B24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EAF632-5E74-8940-8866-A254B571BF35}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="2500" windowWidth="28040" windowHeight="17440" xr2:uid="{835AE8E8-6B96-A741-AB6E-79E0122A2F31}"/>
+    <workbookView xWindow="640" yWindow="4120" windowWidth="26060" windowHeight="22920" xr2:uid="{835AE8E8-6B96-A741-AB6E-79E0122A2F31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>Test</t>
   </si>
@@ -146,9 +146,6 @@
     <t>ParticleTestCase</t>
   </si>
   <si>
-    <t>/LIDARTestCase()</t>
-  </si>
-  <si>
     <t>FindHeightTestCase</t>
   </si>
   <si>
@@ -182,14 +179,44 @@
     <t>Locations seem off sometimes</t>
   </si>
   <si>
-    <t>Labels not working</t>
+    <t>Multi-line not working</t>
+  </si>
+  <si>
+    <t>3D Labels broken.  Probably going to remove them.</t>
+  </si>
+  <si>
+    <t>Needs QuadPagingLayer</t>
+  </si>
+  <si>
+    <t>LIDARTestCase</t>
+  </si>
+  <si>
+    <t>Are the label rotations right?</t>
+  </si>
+  <si>
+    <t>Porting</t>
+  </si>
+  <si>
+    <t>Need to redo elevation support</t>
+  </si>
+  <si>
+    <t>Text looks wrong.  Too blocky.  Also there should be a place name (Belfast), but it's buried</t>
+  </si>
+  <si>
+    <t>SphericalChunkManager turned off</t>
+  </si>
+  <si>
+    <t>Needs snapshot functionality</t>
+  </si>
+  <si>
+    <t>Not working for 2D map (probably z buffer)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +235,20 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -233,10 +274,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +598,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,10 +613,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -588,7 +632,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -596,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -604,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -612,7 +656,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -620,7 +664,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -628,20 +672,26 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -649,10 +699,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -660,7 +710,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -668,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -681,7 +731,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -689,7 +739,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -697,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -705,7 +755,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -713,143 +763,197 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
+      <c r="B23" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B24" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="C28" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C29" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="C31" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C32" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C33" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="C34" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="C35" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C40" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="C43" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got rid of duplicate test case. They all run!  Even if they don't all work.
</commit_message>
<xml_diff>
--- a/TestCaseStatus.xlsx
+++ b/TestCaseStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EAF632-5E74-8940-8866-A254B571BF35}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433CAB17-70E3-3F4A-B679-4AA34AEF381F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="4120" windowWidth="26060" windowHeight="22920" xr2:uid="{835AE8E8-6B96-A741-AB6E-79E0122A2F31}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Test</t>
   </si>
@@ -152,9 +152,6 @@
     <t>FullAnimationTest</t>
   </si>
   <si>
-    <t>ActiveObjectTestCase</t>
-  </si>
-  <si>
     <t>AnimationDelegateTestCase</t>
   </si>
   <si>
@@ -210,6 +207,12 @@
   </si>
   <si>
     <t>Not working for 2D map (probably z buffer)</t>
+  </si>
+  <si>
+    <t>Atmosphere not showing up</t>
+  </si>
+  <si>
+    <t>Has occasional shutdown problems</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F17FF9-7969-3240-AB1E-AD5B8C248AD7}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,10 +616,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -632,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -640,7 +643,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -648,7 +651,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -656,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -664,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -672,7 +675,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -680,10 +683,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -691,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -699,10 +702,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -710,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -718,7 +721,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -731,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -739,7 +742,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -747,7 +750,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -755,7 +758,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -763,7 +766,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -771,10 +774,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -782,7 +785,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -790,7 +793,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -798,10 +801,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,7 +812,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -817,7 +820,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -825,7 +828,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -833,7 +836,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -841,7 +844,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -849,7 +852,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -857,7 +860,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -865,7 +868,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -873,10 +876,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -884,30 +887,42 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -915,45 +930,58 @@
         <v>37</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>38</v>
       </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>39</v>
       </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>43</v>
+      <c r="B50" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Text attribute overrides working again. Colors are right for labels.
</commit_message>
<xml_diff>
--- a/TestCaseStatus.xlsx
+++ b/TestCaseStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433CAB17-70E3-3F4A-B679-4AA34AEF381F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D85CB0-C062-5D4A-A71D-531DCA65C40E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="4120" windowWidth="26060" windowHeight="22920" xr2:uid="{835AE8E8-6B96-A741-AB6E-79E0122A2F31}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>Test</t>
   </si>
@@ -212,14 +212,14 @@
     <t>Atmosphere not showing up</t>
   </si>
   <si>
-    <t>Has occasional shutdown problems</t>
+    <t>Has occasional shutdown problems.  Timer keeps going.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -256,6 +256,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -277,13 +283,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +608,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,9 +731,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Multi-line text working again.
</commit_message>
<xml_diff>
--- a/TestCaseStatus.xlsx
+++ b/TestCaseStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D85CB0-C062-5D4A-A71D-531DCA65C40E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E448E296-9B34-5F4E-B71D-3EEAC0B4AEF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="4120" windowWidth="26060" windowHeight="22920" xr2:uid="{835AE8E8-6B96-A741-AB6E-79E0122A2F31}"/>
   </bookViews>
@@ -176,9 +176,6 @@
     <t>Locations seem off sometimes</t>
   </si>
   <si>
-    <t>Multi-line not working</t>
-  </si>
-  <si>
     <t>3D Labels broken.  Probably going to remove them.</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>Need to redo elevation support</t>
   </si>
   <si>
-    <t>Text looks wrong.  Too blocky.  Also there should be a place name (Belfast), but it's buried</t>
-  </si>
-  <si>
     <t>SphericalChunkManager turned off</t>
   </si>
   <si>
@@ -213,6 +207,12 @@
   </si>
   <si>
     <t>Has occasional shutdown problems.  Timer keeps going.</t>
+  </si>
+  <si>
+    <t>Text looks wrong.  Too blocky.</t>
+  </si>
+  <si>
+    <t>Layout manager not quite right.  Could be layout size.</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,7 +693,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -787,7 +787,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -814,7 +814,7 @@
         <v>45</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -838,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -846,7 +846,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -854,7 +854,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -870,7 +870,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -889,7 +889,7 @@
         <v>45</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,7 +932,7 @@
         <v>45</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -940,15 +940,15 @@
         <v>37</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -983,7 +983,7 @@
         <v>45</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>